<commit_message>
Fixes for new master df format.
</commit_message>
<xml_diff>
--- a/_reference_data/nps_park_dates.xlsx
+++ b/_reference_data/nps_park_dates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="856">
   <si>
     <t>park_name</t>
   </si>
@@ -2425,9 +2425,6 @@
   </si>
   <si>
     <t>Established as part of Hawaii National Park Aug. 1, 1916; renamed Sept. 22, 1961. Boundary changes: May 1, 1922; April 11, 1928; June 20, 1938; Dec. 3, 1940; July 1, 1961; Nov. 10, 1978; Nov. 12, 1998; July 3, 2003. Wilderness designated Nov. 10, 1978. Designated a Biosphere Reserve 1980. Designated a World Heritage Site Dec. 10, 1987.</t>
-  </si>
-  <si>
-    <t>4/20/1832</t>
   </si>
   <si>
     <t>Authorized Nov. 5, 1966. Boundary changes: Oct. 18, 1976; Dec. 28, 1980; Oct. 29, 1986; Oct. 23, 1992.</t>
@@ -2654,9 +2651,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2691,7 +2689,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2702,6 +2700,7 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3035,9 +3034,9 @@
   <dimension ref="A1:F421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="860" topLeftCell="A156" activePane="bottomLeft"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="A172" sqref="A172"/>
+      <pane ySplit="860" topLeftCell="A293" activePane="bottomLeft"/>
+      <selection activeCell="B310" sqref="B310"/>
+      <selection pane="bottomLeft" activeCell="B309" sqref="B309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3746,7 +3745,7 @@
         <v>32</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3877,7 +3876,7 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B59" s="3">
         <v>29504</v>
@@ -5830,7 +5829,7 @@
         <v>470</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="193" spans="1:6" s="8" customFormat="1">
@@ -5988,7 +5987,7 @@
         <v>471</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="202" spans="1:6" s="8" customFormat="1">
@@ -6006,7 +6005,7 @@
         <v>471</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="203" spans="1:6" s="8" customFormat="1">
@@ -6078,7 +6077,7 @@
         <v>471</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="207" spans="1:6" s="8" customFormat="1">
@@ -6204,7 +6203,7 @@
         <v>471</v>
       </c>
       <c r="F213" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="214" spans="1:6" s="8" customFormat="1">
@@ -6600,7 +6599,7 @@
         <v>471</v>
       </c>
       <c r="F235" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="236" spans="1:6" s="8" customFormat="1">
@@ -6816,7 +6815,7 @@
         <v>471</v>
       </c>
       <c r="F247" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="248" spans="1:6" s="8" customFormat="1">
@@ -7158,7 +7157,7 @@
         <v>471</v>
       </c>
       <c r="F266" s="8" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="267" spans="1:6" s="8" customFormat="1">
@@ -7762,7 +7761,7 @@
         <v>472</v>
       </c>
       <c r="F298" s="8" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="299" spans="1:6" s="8" customFormat="1">
@@ -7957,8 +7956,8 @@
       <c r="A309" s="8" t="s">
         <v>670</v>
       </c>
-      <c r="B309" s="9" t="s">
-        <v>802</v>
+      <c r="B309" s="9">
+        <v>7734</v>
       </c>
       <c r="C309" s="9"/>
       <c r="D309" s="9">
@@ -7986,7 +7985,7 @@
         <v>472</v>
       </c>
       <c r="F310" s="8" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="311" spans="1:6" s="8" customFormat="1">
@@ -8004,7 +8003,7 @@
         <v>472</v>
       </c>
       <c r="F311" s="8" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="312" spans="1:6" s="8" customFormat="1">
@@ -8024,7 +8023,7 @@
         <v>472</v>
       </c>
       <c r="F312" s="8" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="313" spans="1:6" s="8" customFormat="1">
@@ -8064,7 +8063,7 @@
         <v>472</v>
       </c>
       <c r="F314" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="315" spans="1:6" s="8" customFormat="1">
@@ -8072,17 +8071,17 @@
         <v>676</v>
       </c>
       <c r="B315" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C315" s="9"/>
       <c r="D315" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E315" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F315" s="8" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="316" spans="1:6" s="8" customFormat="1">
@@ -8102,7 +8101,7 @@
         <v>472</v>
       </c>
       <c r="F316" s="8" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="317" spans="1:6" s="8" customFormat="1">
@@ -8142,7 +8141,7 @@
         <v>472</v>
       </c>
       <c r="F318" s="8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="319" spans="1:6" s="8" customFormat="1">
@@ -8160,7 +8159,7 @@
         <v>472</v>
       </c>
       <c r="F319" s="8" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="320" spans="1:6" s="8" customFormat="1">
@@ -8178,7 +8177,7 @@
         <v>472</v>
       </c>
       <c r="F320" s="8" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="321" spans="1:6" s="8" customFormat="1">
@@ -8186,17 +8185,17 @@
         <v>682</v>
       </c>
       <c r="B321" s="9" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C321" s="9"/>
       <c r="D321" s="9" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E321" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F321" s="8" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="322" spans="1:6" s="8" customFormat="1">
@@ -8214,7 +8213,7 @@
         <v>472</v>
       </c>
       <c r="F322" s="8" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="323" spans="1:6" s="8" customFormat="1">
@@ -8232,7 +8231,7 @@
         <v>472</v>
       </c>
       <c r="F323" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="324" spans="1:6" s="8" customFormat="1">
@@ -8252,7 +8251,7 @@
         <v>472</v>
       </c>
       <c r="F324" s="8" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="325" spans="1:6" s="8" customFormat="1">
@@ -8272,7 +8271,7 @@
         <v>472</v>
       </c>
       <c r="F325" s="8" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="326" spans="1:6" s="8" customFormat="1">
@@ -8292,7 +8291,7 @@
         <v>472</v>
       </c>
       <c r="F326" s="8" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="327" spans="1:6" s="8" customFormat="1">
@@ -8310,7 +8309,7 @@
         <v>472</v>
       </c>
       <c r="F327" s="8" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="328" spans="1:6" s="8" customFormat="1">
@@ -8328,7 +8327,7 @@
         <v>472</v>
       </c>
       <c r="F328" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="329" spans="1:6" s="8" customFormat="1">
@@ -8348,7 +8347,7 @@
         <v>472</v>
       </c>
       <c r="F329" s="8" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="330" spans="1:6" s="8" customFormat="1">
@@ -8356,17 +8355,17 @@
         <v>691</v>
       </c>
       <c r="B330" s="9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C330" s="9"/>
       <c r="D330" s="9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E330" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F330" s="8" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="331" spans="1:6" s="8" customFormat="1">
@@ -8384,7 +8383,7 @@
         <v>472</v>
       </c>
       <c r="F331" s="8" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="332" spans="1:6" s="8" customFormat="1">
@@ -8402,7 +8401,7 @@
         <v>472</v>
       </c>
       <c r="F332" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="333" spans="1:6" s="8" customFormat="1">
@@ -8420,7 +8419,7 @@
         <v>472</v>
       </c>
       <c r="F333" s="8" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="334" spans="1:6" s="8" customFormat="1">
@@ -8438,7 +8437,7 @@
         <v>472</v>
       </c>
       <c r="F334" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="335" spans="1:6" s="8" customFormat="1">
@@ -8456,7 +8455,7 @@
         <v>472</v>
       </c>
       <c r="F335" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="336" spans="1:6" s="8" customFormat="1">
@@ -8484,17 +8483,17 @@
         <v>698</v>
       </c>
       <c r="B337" s="9" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C337" s="9"/>
       <c r="D337" s="9" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E337" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F337" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="338" spans="1:6" s="8" customFormat="1">
@@ -8502,17 +8501,17 @@
         <v>699</v>
       </c>
       <c r="B338" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C338" s="9"/>
       <c r="D338" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E338" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F338" s="8" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="339" spans="1:6" s="8" customFormat="1">
@@ -8532,7 +8531,7 @@
         <v>472</v>
       </c>
       <c r="F339" s="8" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="340" spans="1:6" s="6" customFormat="1">
@@ -8548,7 +8547,7 @@
         <v>473</v>
       </c>
       <c r="F340" s="6" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="341" spans="1:6" s="8" customFormat="1">
@@ -8580,7 +8579,7 @@
         <v>473</v>
       </c>
       <c r="F342" s="8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="343" spans="1:6" s="8" customFormat="1">
@@ -8598,7 +8597,7 @@
         <v>473</v>
       </c>
       <c r="F343" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="344" spans="1:6" s="8" customFormat="1">
@@ -8669,7 +8668,7 @@
         <v>8889</v>
       </c>
       <c r="C348" s="8" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E348" s="8" t="s">
         <v>167</v>
@@ -9522,7 +9521,7 @@
         <v>474</v>
       </c>
       <c r="F401" s="8" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="402" spans="1:6" s="8" customFormat="1">
@@ -9536,7 +9535,7 @@
         <v>474</v>
       </c>
       <c r="F402" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="403" spans="1:6" s="6" customFormat="1">
@@ -9550,7 +9549,7 @@
         <v>474</v>
       </c>
       <c r="F403" s="6" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="404" spans="1:6" s="6" customFormat="1">
@@ -9564,7 +9563,7 @@
         <v>474</v>
       </c>
       <c r="F404" s="6" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="405" spans="1:6" s="8" customFormat="1">
@@ -9578,7 +9577,7 @@
         <v>474</v>
       </c>
       <c r="F405" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="406" spans="1:6" s="8" customFormat="1">
@@ -9592,7 +9591,7 @@
         <v>474</v>
       </c>
       <c r="F406" s="8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="407" spans="1:6" s="6" customFormat="1">
@@ -9606,7 +9605,7 @@
         <v>474</v>
       </c>
       <c r="F407" s="6" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="408" spans="1:6" s="8" customFormat="1">
@@ -9620,7 +9619,7 @@
         <v>474</v>
       </c>
       <c r="F408" s="8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="409" spans="1:6" s="6" customFormat="1">
@@ -9634,7 +9633,7 @@
         <v>474</v>
       </c>
       <c r="F409" s="6" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="410" spans="1:6" s="6" customFormat="1">
@@ -9648,7 +9647,7 @@
         <v>474</v>
       </c>
       <c r="F410" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="411" spans="1:6">

</xml_diff>

<commit_message>
Fix parks file merge.
</commit_message>
<xml_diff>
--- a/_reference_data/nps_park_dates.xlsx
+++ b/_reference_data/nps_park_dates.xlsx
@@ -1935,9 +1935,6 @@
     <t>George Washington Memorial Parkway</t>
   </si>
   <si>
-    <t>John D. Rockefeller</t>
-  </si>
-  <si>
     <t>Natchez Trace Parkway</t>
   </si>
   <si>
@@ -2586,7 +2583,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Martin Luther King National Historical Park</t>
+    <t>John D. Rockefeller National Parkway</t>
+  </si>
+  <si>
+    <t>Martin Luther King National Historic Park</t>
   </si>
 </sst>
 </file>
@@ -3034,8 +3034,8 @@
   <dimension ref="A1:F421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1160" topLeftCell="A290" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F213" sqref="A213:XFD213"/>
+      <pane ySplit="1160" topLeftCell="A44" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3744,7 +3744,7 @@
         <v>32</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -4749,6 +4749,9 @@
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="B120" s="3">
+        <v>14095</v>
+      </c>
       <c r="E120" s="1" t="s">
         <v>88</v>
       </c>
@@ -5828,7 +5831,7 @@
         <v>470</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="193" spans="1:6" s="8" customFormat="1">
@@ -5878,7 +5881,7 @@
         <v>471</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="196" spans="1:6" s="8" customFormat="1">
@@ -5896,7 +5899,7 @@
         <v>471</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="197" spans="1:6" s="8" customFormat="1">
@@ -5914,7 +5917,7 @@
         <v>471</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="198" spans="1:6" s="8" customFormat="1">
@@ -5950,7 +5953,7 @@
         <v>471</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="200" spans="1:6" s="8" customFormat="1">
@@ -5968,7 +5971,7 @@
         <v>471</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="201" spans="1:6" s="8" customFormat="1">
@@ -5986,7 +5989,7 @@
         <v>471</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="202" spans="1:6" s="8" customFormat="1">
@@ -6004,7 +6007,7 @@
         <v>471</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="203" spans="1:6" s="8" customFormat="1">
@@ -6022,7 +6025,7 @@
         <v>471</v>
       </c>
       <c r="F203" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="204" spans="1:6" s="8" customFormat="1">
@@ -6040,7 +6043,7 @@
         <v>471</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="205" spans="1:6" s="8" customFormat="1">
@@ -6058,7 +6061,7 @@
         <v>471</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="206" spans="1:6" s="8" customFormat="1">
@@ -6076,7 +6079,7 @@
         <v>471</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="207" spans="1:6" s="8" customFormat="1">
@@ -6094,7 +6097,7 @@
         <v>471</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="208" spans="1:6" s="8" customFormat="1">
@@ -6112,7 +6115,7 @@
         <v>471</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="209" spans="1:6" s="8" customFormat="1">
@@ -6130,7 +6133,7 @@
         <v>471</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="210" spans="1:6" s="6" customFormat="1">
@@ -6138,17 +6141,17 @@
         <v>557</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D210" s="7"/>
       <c r="E210" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F210" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="211" spans="1:6" s="8" customFormat="1">
@@ -6166,7 +6169,7 @@
         <v>471</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="212" spans="1:6" s="8" customFormat="1">
@@ -6184,7 +6187,7 @@
         <v>471</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="213" spans="1:6" s="6" customFormat="1">
@@ -6202,7 +6205,7 @@
         <v>471</v>
       </c>
       <c r="F213" s="6" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="214" spans="1:6" s="8" customFormat="1">
@@ -6220,7 +6223,7 @@
         <v>471</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="215" spans="1:6" s="8" customFormat="1">
@@ -6238,7 +6241,7 @@
         <v>471</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="216" spans="1:6" s="8" customFormat="1">
@@ -6256,7 +6259,7 @@
         <v>471</v>
       </c>
       <c r="F216" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="217" spans="1:6" s="8" customFormat="1">
@@ -6274,7 +6277,7 @@
         <v>471</v>
       </c>
       <c r="F217" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="218" spans="1:6" s="8" customFormat="1">
@@ -6292,7 +6295,7 @@
         <v>471</v>
       </c>
       <c r="F218" s="8" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="219" spans="1:6" s="8" customFormat="1">
@@ -6328,7 +6331,7 @@
         <v>471</v>
       </c>
       <c r="F220" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="221" spans="1:6" s="8" customFormat="1">
@@ -6346,7 +6349,7 @@
         <v>471</v>
       </c>
       <c r="F221" s="8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="222" spans="1:6" s="8" customFormat="1">
@@ -6364,7 +6367,7 @@
         <v>471</v>
       </c>
       <c r="F222" s="8" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="223" spans="1:6" s="8" customFormat="1">
@@ -6382,7 +6385,7 @@
         <v>471</v>
       </c>
       <c r="F223" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="224" spans="1:6" s="8" customFormat="1">
@@ -6400,7 +6403,7 @@
         <v>471</v>
       </c>
       <c r="F224" s="8" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="225" spans="1:6" s="8" customFormat="1">
@@ -6418,7 +6421,7 @@
         <v>471</v>
       </c>
       <c r="F225" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="226" spans="1:6" s="8" customFormat="1">
@@ -6436,7 +6439,7 @@
         <v>471</v>
       </c>
       <c r="F226" s="8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="227" spans="1:6" s="8" customFormat="1">
@@ -6454,7 +6457,7 @@
         <v>471</v>
       </c>
       <c r="F227" s="8" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="228" spans="1:6" s="8" customFormat="1">
@@ -6472,7 +6475,7 @@
         <v>471</v>
       </c>
       <c r="F228" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="229" spans="1:6" s="8" customFormat="1">
@@ -6490,7 +6493,7 @@
         <v>471</v>
       </c>
       <c r="F229" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="230" spans="1:6" s="8" customFormat="1">
@@ -6508,7 +6511,7 @@
         <v>471</v>
       </c>
       <c r="F230" s="8" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="231" spans="1:6" s="8" customFormat="1">
@@ -6526,7 +6529,7 @@
         <v>471</v>
       </c>
       <c r="F231" s="8" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="232" spans="1:6" s="8" customFormat="1">
@@ -6544,7 +6547,7 @@
         <v>471</v>
       </c>
       <c r="F232" s="8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="233" spans="1:6" s="8" customFormat="1">
@@ -6562,7 +6565,7 @@
         <v>471</v>
       </c>
       <c r="F233" s="8" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="234" spans="1:6" s="8" customFormat="1">
@@ -6580,7 +6583,7 @@
         <v>471</v>
       </c>
       <c r="F234" s="8" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="235" spans="1:6" s="8" customFormat="1">
@@ -6598,7 +6601,7 @@
         <v>471</v>
       </c>
       <c r="F235" s="8" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="236" spans="1:6" s="8" customFormat="1">
@@ -6616,7 +6619,7 @@
         <v>471</v>
       </c>
       <c r="F236" s="8" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="237" spans="1:6" s="8" customFormat="1">
@@ -6634,7 +6637,7 @@
         <v>471</v>
       </c>
       <c r="F237" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="238" spans="1:6" s="8" customFormat="1">
@@ -6652,7 +6655,7 @@
         <v>471</v>
       </c>
       <c r="F238" s="8" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="239" spans="1:6" s="8" customFormat="1">
@@ -6670,7 +6673,7 @@
         <v>471</v>
       </c>
       <c r="F239" s="8" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="240" spans="1:6" s="6" customFormat="1">
@@ -6688,7 +6691,7 @@
         <v>471</v>
       </c>
       <c r="F240" s="6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="241" spans="1:6" s="8" customFormat="1">
@@ -6706,7 +6709,7 @@
         <v>471</v>
       </c>
       <c r="F241" s="8" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="242" spans="1:6" s="8" customFormat="1">
@@ -6724,7 +6727,7 @@
         <v>471</v>
       </c>
       <c r="F242" s="8" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="243" spans="1:6" s="8" customFormat="1">
@@ -6742,7 +6745,7 @@
         <v>471</v>
       </c>
       <c r="F243" s="8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="244" spans="1:6" s="8" customFormat="1">
@@ -6760,7 +6763,7 @@
         <v>471</v>
       </c>
       <c r="F244" s="8" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="245" spans="1:6" s="8" customFormat="1">
@@ -6778,7 +6781,7 @@
         <v>471</v>
       </c>
       <c r="F245" s="8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="246" spans="1:6" s="8" customFormat="1">
@@ -6796,7 +6799,7 @@
         <v>471</v>
       </c>
       <c r="F246" s="8" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="247" spans="1:6" s="8" customFormat="1">
@@ -6814,7 +6817,7 @@
         <v>471</v>
       </c>
       <c r="F247" s="8" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="248" spans="1:6" s="8" customFormat="1">
@@ -6832,7 +6835,7 @@
         <v>471</v>
       </c>
       <c r="F248" s="8" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="249" spans="1:6" s="6" customFormat="1">
@@ -6840,7 +6843,7 @@
         <v>596</v>
       </c>
       <c r="B249" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C249" s="7">
         <v>16883</v>
@@ -6850,7 +6853,7 @@
         <v>471</v>
       </c>
       <c r="F249" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="250" spans="1:6" s="8" customFormat="1">
@@ -6868,7 +6871,7 @@
         <v>471</v>
       </c>
       <c r="F250" s="8" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="251" spans="1:6" s="8" customFormat="1">
@@ -6886,7 +6889,7 @@
         <v>471</v>
       </c>
       <c r="F251" s="8" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="252" spans="1:6" s="8" customFormat="1">
@@ -6904,7 +6907,7 @@
         <v>471</v>
       </c>
       <c r="F252" s="8" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="253" spans="1:6" s="8" customFormat="1">
@@ -6922,7 +6925,7 @@
         <v>471</v>
       </c>
       <c r="F253" s="8" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="254" spans="1:6" s="8" customFormat="1">
@@ -6940,7 +6943,7 @@
         <v>471</v>
       </c>
       <c r="F254" s="8" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="255" spans="1:6" s="8" customFormat="1">
@@ -6958,7 +6961,7 @@
         <v>471</v>
       </c>
       <c r="F255" s="8" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="256" spans="1:6" s="8" customFormat="1">
@@ -6976,7 +6979,7 @@
         <v>471</v>
       </c>
       <c r="F256" s="8" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="257" spans="1:6" s="8" customFormat="1">
@@ -6994,7 +6997,7 @@
         <v>471</v>
       </c>
       <c r="F257" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="258" spans="1:6" s="8" customFormat="1">
@@ -7012,7 +7015,7 @@
         <v>471</v>
       </c>
       <c r="F258" s="8" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="259" spans="1:6" s="8" customFormat="1">
@@ -7030,7 +7033,7 @@
         <v>471</v>
       </c>
       <c r="F259" s="8" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="260" spans="1:6" s="8" customFormat="1">
@@ -7048,7 +7051,7 @@
         <v>471</v>
       </c>
       <c r="F260" s="8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="261" spans="1:6" s="8" customFormat="1">
@@ -7066,7 +7069,7 @@
         <v>471</v>
       </c>
       <c r="F261" s="8" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="262" spans="1:6" s="8" customFormat="1">
@@ -7084,7 +7087,7 @@
         <v>471</v>
       </c>
       <c r="F262" s="8" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="263" spans="1:6" s="8" customFormat="1">
@@ -7102,7 +7105,7 @@
         <v>471</v>
       </c>
       <c r="F263" s="8" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="264" spans="1:6" s="8" customFormat="1">
@@ -7120,7 +7123,7 @@
         <v>471</v>
       </c>
       <c r="F264" s="8" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="265" spans="1:6" s="8" customFormat="1">
@@ -7138,7 +7141,7 @@
         <v>471</v>
       </c>
       <c r="F265" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="266" spans="1:6" s="8" customFormat="1">
@@ -7156,7 +7159,7 @@
         <v>471</v>
       </c>
       <c r="F266" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="267" spans="1:6" s="8" customFormat="1">
@@ -7174,7 +7177,7 @@
         <v>471</v>
       </c>
       <c r="F267" s="8" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="268" spans="1:6" s="8" customFormat="1">
@@ -7192,7 +7195,7 @@
         <v>471</v>
       </c>
       <c r="F268" s="8" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="269" spans="1:6" s="8" customFormat="1">
@@ -7210,7 +7213,7 @@
         <v>471</v>
       </c>
       <c r="F269" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="270" spans="1:6" s="8" customFormat="1">
@@ -7264,7 +7267,7 @@
         <v>471</v>
       </c>
       <c r="F272" s="8" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="273" spans="1:6" s="8" customFormat="1">
@@ -7282,7 +7285,7 @@
         <v>471</v>
       </c>
       <c r="F273" s="8" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="274" spans="1:6" s="8" customFormat="1">
@@ -7300,7 +7303,7 @@
         <v>471</v>
       </c>
       <c r="F274" s="8" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="275" spans="1:6" s="8" customFormat="1">
@@ -7318,7 +7321,7 @@
         <v>471</v>
       </c>
       <c r="F275" s="8" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="276" spans="1:6" s="8" customFormat="1">
@@ -7336,7 +7339,7 @@
         <v>471</v>
       </c>
       <c r="F276" s="8" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="277" spans="1:6" s="8" customFormat="1">
@@ -7354,7 +7357,7 @@
         <v>471</v>
       </c>
       <c r="F277" s="8" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="278" spans="1:6" s="8" customFormat="1">
@@ -7372,12 +7375,12 @@
         <v>471</v>
       </c>
       <c r="F278" s="8" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="279" spans="1:6" s="8" customFormat="1">
       <c r="A279" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B279" s="9">
         <v>6034</v>
@@ -7392,12 +7395,12 @@
         <v>472</v>
       </c>
       <c r="F279" s="8" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="280" spans="1:6" s="8" customFormat="1">
       <c r="A280" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B280" s="9">
         <v>10695</v>
@@ -7412,12 +7415,12 @@
         <v>472</v>
       </c>
       <c r="F280" s="8" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="281" spans="1:6" s="8" customFormat="1">
       <c r="A281" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B281" s="9">
         <v>10656</v>
@@ -7432,12 +7435,12 @@
         <v>472</v>
       </c>
       <c r="F281" s="8" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="282" spans="1:6" s="8" customFormat="1">
       <c r="A282" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B282" s="9">
         <v>16235</v>
@@ -7450,12 +7453,12 @@
         <v>472</v>
       </c>
       <c r="F282" s="8" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="283" spans="1:6" s="8" customFormat="1">
       <c r="A283" s="8" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B283" s="9">
         <v>25129</v>
@@ -7470,12 +7473,12 @@
         <v>472</v>
       </c>
       <c r="F283" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="284" spans="1:6" s="8" customFormat="1">
       <c r="A284" s="8" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B284" s="9">
         <v>12115</v>
@@ -7490,12 +7493,12 @@
         <v>472</v>
       </c>
       <c r="F284" s="8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="285" spans="1:6" s="8" customFormat="1">
       <c r="A285" s="8" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B285" s="9">
         <v>8560</v>
@@ -7510,12 +7513,12 @@
         <v>472</v>
       </c>
       <c r="F285" s="8" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="286" spans="1:6" s="8" customFormat="1">
       <c r="A286" s="8" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B286" s="9">
         <v>23632</v>
@@ -7528,12 +7531,12 @@
         <v>472</v>
       </c>
       <c r="F286" s="8" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="287" spans="1:6" s="8" customFormat="1">
       <c r="A287" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B287" s="9">
         <v>13729</v>
@@ -7548,12 +7551,12 @@
         <v>472</v>
       </c>
       <c r="F287" s="8" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="288" spans="1:6" s="8" customFormat="1">
       <c r="A288" s="8" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B288" s="9">
         <v>8699</v>
@@ -7568,12 +7571,12 @@
         <v>472</v>
       </c>
       <c r="F288" s="8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="289" spans="1:6" s="8" customFormat="1">
       <c r="A289" s="8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B289" s="9">
         <v>13996</v>
@@ -7588,12 +7591,12 @@
         <v>472</v>
       </c>
       <c r="F289" s="8" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="290" spans="1:6" s="8" customFormat="1">
       <c r="A290" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B290" s="9">
         <v>28051</v>
@@ -7608,12 +7611,12 @@
         <v>472</v>
       </c>
       <c r="F290" s="8" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="291" spans="1:6" s="8" customFormat="1">
       <c r="A291" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B291" s="9">
         <v>873</v>
@@ -7626,12 +7629,12 @@
         <v>472</v>
       </c>
       <c r="F291" s="8" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="292" spans="1:6" s="8" customFormat="1">
       <c r="A292" s="8" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B292" s="9">
         <v>27390</v>
@@ -7644,12 +7647,12 @@
         <v>472</v>
       </c>
       <c r="F292" s="8" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="293" spans="1:6" s="8" customFormat="1">
       <c r="A293" s="8" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B293" s="9">
         <v>12096</v>
@@ -7664,12 +7667,12 @@
         <v>472</v>
       </c>
       <c r="F293" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="294" spans="1:6" s="8" customFormat="1">
       <c r="A294" s="8" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B294" s="9">
         <v>6267</v>
@@ -7689,7 +7692,7 @@
     </row>
     <row r="295" spans="1:6" s="8" customFormat="1">
       <c r="A295" s="8" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B295" s="9">
         <v>12788</v>
@@ -7704,12 +7707,12 @@
         <v>472</v>
       </c>
       <c r="F295" s="8" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="296" spans="1:6" s="8" customFormat="1">
       <c r="A296" s="8" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B296" s="9">
         <v>12569</v>
@@ -7722,12 +7725,12 @@
         <v>472</v>
       </c>
       <c r="F296" s="8" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="297" spans="1:6" s="8" customFormat="1">
       <c r="A297" s="8" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B297" s="9">
         <v>28825</v>
@@ -7747,7 +7750,7 @@
     </row>
     <row r="298" spans="1:6" s="8" customFormat="1">
       <c r="A298" s="8" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B298" s="9">
         <v>13139</v>
@@ -7760,12 +7763,12 @@
         <v>472</v>
       </c>
       <c r="F298" s="8" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="299" spans="1:6" s="8" customFormat="1">
       <c r="A299" s="8" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B299" s="9">
         <v>9189</v>
@@ -7785,7 +7788,7 @@
     </row>
     <row r="300" spans="1:6" s="8" customFormat="1">
       <c r="A300" s="8" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B300" s="9">
         <v>3784</v>
@@ -7798,12 +7801,12 @@
         <v>472</v>
       </c>
       <c r="F300" s="8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="301" spans="1:6" s="8" customFormat="1">
       <c r="A301" s="8" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B301" s="9" t="s">
         <v>433</v>
@@ -7818,12 +7821,12 @@
         <v>472</v>
       </c>
       <c r="F301" s="8" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="302" spans="1:6" s="8" customFormat="1">
       <c r="A302" s="8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B302" s="9">
         <v>10650</v>
@@ -7836,12 +7839,12 @@
         <v>472</v>
       </c>
       <c r="F302" s="8" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="303" spans="1:6" s="8" customFormat="1">
       <c r="A303" s="8" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B303" s="9">
         <v>8060</v>
@@ -7856,12 +7859,12 @@
         <v>472</v>
       </c>
       <c r="F303" s="8" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="304" spans="1:6" s="8" customFormat="1">
       <c r="A304" s="8" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B304" s="9">
         <v>11765</v>
@@ -7881,7 +7884,7 @@
     </row>
     <row r="305" spans="1:6" s="8" customFormat="1">
       <c r="A305" s="8" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B305" s="9">
         <v>9639</v>
@@ -7894,12 +7897,12 @@
         <v>472</v>
       </c>
       <c r="F305" s="8" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="306" spans="1:6" s="8" customFormat="1">
       <c r="A306" s="8" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B306" s="9">
         <v>26572</v>
@@ -7912,12 +7915,12 @@
         <v>472</v>
       </c>
       <c r="F306" s="8" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="307" spans="1:6" s="8" customFormat="1">
       <c r="A307" s="8" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B307" s="9">
         <v>6058</v>
@@ -7930,12 +7933,12 @@
         <v>472</v>
       </c>
       <c r="F307" s="8" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="308" spans="1:6" s="8" customFormat="1">
       <c r="A308" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B308" s="9">
         <v>6058</v>
@@ -7948,12 +7951,12 @@
         <v>472</v>
       </c>
       <c r="F308" s="8" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="309" spans="1:6" s="6" customFormat="1">
       <c r="A309" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B309" s="7">
         <v>7734</v>
@@ -7966,12 +7969,12 @@
         <v>472</v>
       </c>
       <c r="F309" s="6" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="310" spans="1:6" s="8" customFormat="1">
       <c r="A310" s="8" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B310" s="9">
         <v>24416</v>
@@ -7984,12 +7987,12 @@
         <v>472</v>
       </c>
       <c r="F310" s="8" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="311" spans="1:6" s="8" customFormat="1">
       <c r="A311" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B311" s="9">
         <v>11385</v>
@@ -8002,12 +8005,12 @@
         <v>472</v>
       </c>
       <c r="F311" s="8" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="312" spans="1:6" s="8" customFormat="1">
       <c r="A312" s="8" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B312" s="9">
         <v>13372</v>
@@ -8022,12 +8025,12 @@
         <v>472</v>
       </c>
       <c r="F312" s="8" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="313" spans="1:6" s="8" customFormat="1">
       <c r="A313" s="8" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B313" s="9">
         <v>6842</v>
@@ -8047,7 +8050,7 @@
     </row>
     <row r="314" spans="1:6" s="8" customFormat="1">
       <c r="A314" s="8" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B314" s="9">
         <v>28825</v>
@@ -8062,30 +8065,30 @@
         <v>472</v>
       </c>
       <c r="F314" s="8" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="315" spans="1:6" s="8" customFormat="1">
       <c r="A315" s="8" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B315" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C315" s="9"/>
       <c r="D315" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E315" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F315" s="8" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="316" spans="1:6" s="8" customFormat="1">
       <c r="A316" s="8" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B316" s="9">
         <v>28825</v>
@@ -8100,12 +8103,12 @@
         <v>472</v>
       </c>
       <c r="F316" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="317" spans="1:6" s="8" customFormat="1">
       <c r="A317" s="8" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B317" s="9">
         <v>28825</v>
@@ -8125,7 +8128,7 @@
     </row>
     <row r="318" spans="1:6" s="8" customFormat="1">
       <c r="A318" s="8" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B318" s="9">
         <v>2683</v>
@@ -8140,12 +8143,12 @@
         <v>472</v>
       </c>
       <c r="F318" s="8" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="319" spans="1:6" s="8" customFormat="1">
       <c r="A319" s="8" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B319" s="9">
         <v>9642</v>
@@ -8158,12 +8161,12 @@
         <v>472</v>
       </c>
       <c r="F319" s="8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="320" spans="1:6" s="8" customFormat="1">
       <c r="A320" s="8" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B320" s="9">
         <v>2372</v>
@@ -8176,30 +8179,30 @@
         <v>472</v>
       </c>
       <c r="F320" s="8" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="321" spans="1:6" s="8" customFormat="1">
       <c r="A321" s="8" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B321" s="9" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C321" s="9"/>
       <c r="D321" s="9" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E321" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F321" s="8" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="322" spans="1:6" s="8" customFormat="1">
       <c r="A322" s="8" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B322" s="9">
         <v>32447</v>
@@ -8212,12 +8215,12 @@
         <v>472</v>
       </c>
       <c r="F322" s="8" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="323" spans="1:6" s="8" customFormat="1">
       <c r="A323" s="8" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B323" s="9">
         <v>25113</v>
@@ -8230,12 +8233,12 @@
         <v>472</v>
       </c>
       <c r="F323" s="8" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="324" spans="1:6" s="8" customFormat="1">
       <c r="A324" s="8" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B324" s="9">
         <v>3349</v>
@@ -8250,12 +8253,12 @@
         <v>472</v>
       </c>
       <c r="F324" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="325" spans="1:6" s="8" customFormat="1">
       <c r="A325" s="8" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B325" s="9">
         <v>2534</v>
@@ -8270,12 +8273,12 @@
         <v>472</v>
       </c>
       <c r="F325" s="8" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="326" spans="1:6" s="8" customFormat="1">
       <c r="A326" s="8" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B326" s="9">
         <v>2938</v>
@@ -8290,12 +8293,12 @@
         <v>472</v>
       </c>
       <c r="F326" s="8" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="327" spans="1:6" s="8" customFormat="1">
       <c r="A327" s="8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B327" s="9">
         <v>25113</v>
@@ -8308,12 +8311,12 @@
         <v>472</v>
       </c>
       <c r="F327" s="8" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="328" spans="1:6" s="8" customFormat="1">
       <c r="A328" s="8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B328" s="9">
         <v>5505</v>
@@ -8326,12 +8329,12 @@
         <v>472</v>
       </c>
       <c r="F328" s="8" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="329" spans="1:6" s="8" customFormat="1">
       <c r="A329" s="8" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B329" s="9">
         <v>12114</v>
@@ -8346,30 +8349,30 @@
         <v>472</v>
       </c>
       <c r="F329" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="330" spans="1:6" s="8" customFormat="1">
       <c r="A330" s="8" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B330" s="9" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C330" s="9"/>
       <c r="D330" s="9" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E330" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F330" s="8" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="331" spans="1:6" s="8" customFormat="1">
       <c r="A331" s="8" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B331" s="9">
         <v>9639</v>
@@ -8382,12 +8385,12 @@
         <v>472</v>
       </c>
       <c r="F331" s="8" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="332" spans="1:6" s="8" customFormat="1">
       <c r="A332" s="8" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B332" s="9">
         <v>17282</v>
@@ -8400,12 +8403,12 @@
         <v>472</v>
       </c>
       <c r="F332" s="8" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="333" spans="1:6" s="8" customFormat="1">
       <c r="A333" s="8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B333" s="9">
         <v>20669</v>
@@ -8418,12 +8421,12 @@
         <v>472</v>
       </c>
       <c r="F333" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="334" spans="1:6" s="8" customFormat="1">
       <c r="A334" s="8" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B334" s="9">
         <v>25941</v>
@@ -8436,12 +8439,12 @@
         <v>472</v>
       </c>
       <c r="F334" s="8" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="335" spans="1:6" s="8" customFormat="1">
       <c r="A335" s="8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B335" s="9">
         <v>1105</v>
@@ -8454,12 +8457,12 @@
         <v>472</v>
       </c>
       <c r="F335" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="336" spans="1:6" s="8" customFormat="1">
       <c r="A336" s="8" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B336" s="9">
         <v>28825</v>
@@ -8479,43 +8482,43 @@
     </row>
     <row r="337" spans="1:6" s="8" customFormat="1">
       <c r="A337" s="8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B337" s="9" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C337" s="9"/>
       <c r="D337" s="9" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E337" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F337" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="338" spans="1:6" s="8" customFormat="1">
       <c r="A338" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B338" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C338" s="9"/>
       <c r="D338" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E338" s="8" t="s">
         <v>472</v>
       </c>
       <c r="F338" s="8" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="339" spans="1:6" s="8" customFormat="1">
       <c r="A339" s="8" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B339" s="9">
         <v>3500</v>
@@ -8530,7 +8533,7 @@
         <v>472</v>
       </c>
       <c r="F339" s="8" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="340" spans="1:6" s="6" customFormat="1">
@@ -8546,7 +8549,7 @@
         <v>473</v>
       </c>
       <c r="F340" s="6" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="341" spans="1:6" s="8" customFormat="1">
@@ -8567,7 +8570,7 @@
     </row>
     <row r="342" spans="1:6" s="8" customFormat="1">
       <c r="A342" s="8" t="s">
-        <v>638</v>
+        <v>854</v>
       </c>
       <c r="B342" s="9">
         <v>26536</v>
@@ -8578,12 +8581,12 @@
         <v>473</v>
       </c>
       <c r="F342" s="8" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="343" spans="1:6" s="8" customFormat="1">
       <c r="A343" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B343" s="9">
         <v>14018</v>
@@ -8596,7 +8599,7 @@
         <v>473</v>
       </c>
       <c r="F343" s="8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="344" spans="1:6" s="8" customFormat="1">
@@ -8667,7 +8670,7 @@
         <v>8889</v>
       </c>
       <c r="C348" s="8" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E348" s="8" t="s">
         <v>167</v>
@@ -9518,7 +9521,7 @@
         <v>474</v>
       </c>
       <c r="F401" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="402" spans="1:6" s="8" customFormat="1">
@@ -9532,7 +9535,7 @@
         <v>474</v>
       </c>
       <c r="F402" s="8" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="403" spans="1:6" s="6" customFormat="1">
@@ -9546,7 +9549,7 @@
         <v>474</v>
       </c>
       <c r="F403" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="404" spans="1:6" s="6" customFormat="1">
@@ -9560,7 +9563,7 @@
         <v>474</v>
       </c>
       <c r="F404" s="6" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="405" spans="1:6" s="8" customFormat="1">
@@ -9574,7 +9577,7 @@
         <v>474</v>
       </c>
       <c r="F405" s="8" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="406" spans="1:6" s="8" customFormat="1">
@@ -9588,7 +9591,7 @@
         <v>474</v>
       </c>
       <c r="F406" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="407" spans="1:6" s="6" customFormat="1">
@@ -9602,7 +9605,7 @@
         <v>474</v>
       </c>
       <c r="F407" s="6" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="408" spans="1:6" s="8" customFormat="1">
@@ -9616,7 +9619,7 @@
         <v>474</v>
       </c>
       <c r="F408" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="409" spans="1:6" s="6" customFormat="1">
@@ -9630,7 +9633,7 @@
         <v>474</v>
       </c>
       <c r="F409" s="6" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="410" spans="1:6" s="6" customFormat="1">
@@ -9644,7 +9647,7 @@
         <v>474</v>
       </c>
       <c r="F410" s="6" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="411" spans="1:6">

</xml_diff>